<commit_message>
Tracking another day of exports
</commit_message>
<xml_diff>
--- a/exportTracker.xlsx
+++ b/exportTracker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="226">
   <si>
     <t>List of MRC Pages with jQuery Fixes</t>
   </si>
@@ -691,6 +691,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run problem ones through a linter a second time? </t>
   </si>
 </sst>
 </file>
@@ -1052,11 +1055,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F222"/>
+  <dimension ref="B1:G222"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B81" sqref="B81"/>
+      <selection pane="bottomLeft" activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,7 +1067,7 @@
     <col min="2" max="2" width="56.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1073,17 +1076,20 @@
       </c>
       <c r="D1">
         <f>COUNTIF(C2:C300,"x")</f>
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E1" t="s">
         <v>223</v>
       </c>
       <c r="F1">
         <f>COUNTIF(E2:E300,"x")</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1091,7 +1097,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1099,7 +1105,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1107,7 +1113,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1115,7 +1121,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1123,7 +1129,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1131,7 +1137,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1139,7 +1145,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1147,7 +1153,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1155,7 +1161,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
@@ -1163,7 +1169,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
@@ -1171,7 +1177,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
@@ -1179,7 +1185,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1187,7 +1193,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1195,7 +1201,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
@@ -1715,82 +1721,106 @@
         <v>224</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="E82" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="E83" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="E86" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C87" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
         <v>95</v>
       </c>
@@ -2511,7 +2541,7 @@
     <hyperlink ref="B83" r:id="rId82" display="http://localhost:8080/03_jQuery-Test/Frenchfilm.html"/>
     <hyperlink ref="B84" r:id="rId83" display="http://localhost:8080/03_jQuery-Test/frizfreleng.html"/>
     <hyperlink ref="B85" r:id="rId84" display="http://localhost:8080/03_jQuery-Test/FSM.html"/>
-    <hyperlink ref="B86" r:id="rId85" display="http://localhost:8080/03_jQuery-Test/Gangsterfilm.html"/>
+    <hyperlink ref="B86" r:id="rId85"/>
     <hyperlink ref="B87" r:id="rId86" display="http://localhost:8080/03_jQuery-Test/GayVid.html"/>
     <hyperlink ref="B88" r:id="rId87" display="http://localhost:8080/03_jQuery-Test/GayVid2.html"/>
     <hyperlink ref="B89" r:id="rId88" display="http://localhost:8080/03_jQuery-Test/germanculture.html"/>

</xml_diff>

<commit_message>
Final Work Day Commit!
</commit_message>
<xml_diff>
--- a/exportTracker.xlsx
+++ b/exportTracker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="226">
   <si>
     <t>List of MRC Pages with jQuery Fixes</t>
   </si>
@@ -1058,8 +1058,8 @@
   <dimension ref="B1:G222"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C88" sqref="C88"/>
+      <pane ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B125" sqref="B125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1076,14 +1076,14 @@
       </c>
       <c r="D1">
         <f>COUNTIF(C2:C300,"x")</f>
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="E1" t="s">
         <v>223</v>
       </c>
       <c r="F1">
         <f>COUNTIF(E2:E300,"x")</f>
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
         <v>225</v>
@@ -1789,198 +1789,306 @@
       <c r="B89" s="2" t="s">
         <v>88</v>
       </c>
+      <c r="E89" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
         <v>89</v>
       </c>
+      <c r="E90" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="91" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
         <v>90</v>
       </c>
+      <c r="C91" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
         <v>91</v>
       </c>
+      <c r="E92" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="93" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
         <v>92</v>
       </c>
+      <c r="C93" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="94" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
         <v>93</v>
       </c>
+      <c r="E94" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
         <v>94</v>
       </c>
+      <c r="E95" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C96" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C97" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="E98" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C99" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B100" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C100" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B101" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C101" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B102" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C102" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B103" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C103" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B104" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C104" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B105" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C105" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B106" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C106" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B107" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C107" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C108" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B109" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C109" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B110" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="E110" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B111" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="E111" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="112" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B112" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C112" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B113" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C113" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B114" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C114" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B115" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C115" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B116" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C116" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C117" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B118" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C118" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B119" s="2" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C119" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="120" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B120" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="E120" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="121" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B121" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="E121" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="122" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B122" s="2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C122" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="123" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B123" s="2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C123" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B124" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="E124" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="125" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B125" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B126" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B127" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B128" s="2" t="s">
         <v>127</v>
       </c>

</xml_diff>